<commit_message>
[M] rename data_of_2022-01-07 to data_of_2022-01-07_old, and add eval_system.xlsx
</commit_message>
<xml_diff>
--- a/out/ml_model_result/index_ml_model_result.xlsx
+++ b/out/ml_model_result/index_ml_model_result.xlsx
@@ -1,25 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toranosuke/Desktop/DoV_ML/out/ml_model_result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{64D8F897-C859-7841-A0AE-561647285BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{1B9CEEDA-522D-DC40-8E22-F850B2FBFCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="500" yWindow="500" windowWidth="34640" windowHeight="21100" xr2:uid="{C39C54D5-2076-D54E-9F47-FB65B7F2F040}"/>
+    <workbookView xWindow="-35680" yWindow="500" windowWidth="34640" windowHeight="21100" xr2:uid="{C39C54D5-2076-D54E-9F47-FB65B7F2F040}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$49</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$56</definedName>
     <definedName name="Z_0848F74C_49F2_314A_990A_863A30F08478_.wvu.FilterData" localSheetId="0" hidden="1">Sheet1!$A$1:$K$49</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <customWorkbookViews>
     <customWorkbookView name="加藤虎之介 - 個人用ビュー" guid="{0848F74C-49F2-314A-990A-863A30F08478}" mergeInterval="0" personalView="1" xWindow="25" yWindow="25" windowWidth="1732" windowHeight="1055" activeSheetId="1"/>
   </customWorkbookViews>
@@ -245,10 +245,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Facing Angles</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Accuracy</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -381,6 +377,10 @@
     <rPh sb="6" eb="8">
       <t>チャク</t>
     </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Facing Angle</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -571,8 +571,8 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{A0F87F0E-2EF0-0F41-ABD3-D04FE472377F}" diskRevisions="1" revisionId="114" version="10">
-  <header guid="{A0F87F0E-2EF0-0F41-ABD3-D04FE472377F}" dateTime="2021-12-07T15:04:57" maxSheetId="2" userName="加藤虎之介" r:id="rId10" minRId="109" maxRId="114">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{8B03C332-5321-3549-9B40-9AF02F64FAC3}" diskRevisions="1" revisionId="115" version="11">
+  <header guid="{8B03C332-5321-3549-9B40-9AF02F64FAC3}" dateTime="2022-01-21T14:43:48" maxSheetId="2" userName="加藤虎之介" r:id="rId11" minRId="115">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -580,43 +580,18 @@
 </headers>
 </file>
 
-<file path=xl/revisions/revisionLog10.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <rcc rId="109" sId="1">
-    <nc r="C54" t="b">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcc rId="110" sId="1">
-    <nc r="C55" t="b">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcc rId="111" sId="1">
-    <nc r="C56" t="b">
-      <v>0</v>
-    </nc>
-  </rcc>
-  <rcc rId="112" sId="1">
-    <nc r="E54" t="inlineStr">
+  <rcc rId="115" sId="1">
+    <oc r="D1" t="inlineStr">
       <is>
-        <t>2021-11-29_mac_48000Hz_w1_N2^12_overlap80.csv</t>
+        <t>Facing Angles</t>
         <phoneticPr fontId="0"/>
       </is>
-    </nc>
-  </rcc>
-  <rcc rId="113" sId="1">
-    <nc r="E55" t="inlineStr">
+    </oc>
+    <nc r="D1" t="inlineStr">
       <is>
-        <t>2021-11-26_raspi_16000Hz_w1_N2^12_overlap80.csv</t>
-        <phoneticPr fontId="0"/>
-      </is>
-    </nc>
-  </rcc>
-  <rcc rId="114" sId="1">
-    <nc r="E56" t="inlineStr">
-      <is>
-        <t>2021-11-29_mac_48000Hz_w1_N2^12_overlap80.csv</t>
+        <t>Facing Angle</t>
         <phoneticPr fontId="0"/>
       </is>
     </nc>
@@ -928,8 +903,8 @@
   <dimension ref="A1:K1048575"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -948,30 +923,30 @@
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1">
       <c r="A1" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B1" s="22" t="s">
         <v>39</v>
       </c>
       <c r="C1" s="21" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D1" s="23" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="E1" s="22" t="s">
         <v>48</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G1" s="22"/>
       <c r="H1" s="22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I1" s="22"/>
       <c r="J1" s="22" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K1" s="22"/>
     </row>
@@ -982,27 +957,27 @@
       <c r="D2" s="23"/>
       <c r="E2" s="22"/>
       <c r="F2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="18" customFormat="1">
       <c r="A3" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3" s="18" t="s">
         <v>0</v>
@@ -1011,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E3" s="18" t="s">
         <v>49</v>
@@ -1037,7 +1012,7 @@
     </row>
     <row r="4" spans="1:11" s="18" customFormat="1">
       <c r="A4" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>1</v>
@@ -1046,7 +1021,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E4" s="18" t="s">
         <v>50</v>
@@ -1072,7 +1047,7 @@
     </row>
     <row r="5" spans="1:11" s="18" customFormat="1">
       <c r="A5" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>2</v>
@@ -1081,7 +1056,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>49</v>
@@ -1107,7 +1082,7 @@
     </row>
     <row r="6" spans="1:11" s="18" customFormat="1">
       <c r="A6" s="18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>3</v>
@@ -1116,7 +1091,7 @@
         <v>0</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>50</v>
@@ -1142,7 +1117,7 @@
     </row>
     <row r="7" spans="1:11" s="13" customFormat="1">
       <c r="A7" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>4</v>
@@ -1151,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>49</v>
@@ -1177,7 +1152,7 @@
     </row>
     <row r="8" spans="1:11" s="13" customFormat="1">
       <c r="A8" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B8" s="13" t="s">
         <v>5</v>
@@ -1186,7 +1161,7 @@
         <v>0</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>50</v>
@@ -1212,7 +1187,7 @@
     </row>
     <row r="9" spans="1:11" s="13" customFormat="1">
       <c r="A9" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B9" s="13" t="s">
         <v>6</v>
@@ -1221,7 +1196,7 @@
         <v>0</v>
       </c>
       <c r="D9" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>49</v>
@@ -1247,7 +1222,7 @@
     </row>
     <row r="10" spans="1:11" s="13" customFormat="1">
       <c r="A10" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B10" s="13" t="s">
         <v>7</v>
@@ -1256,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="D10" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E10" s="13" t="s">
         <v>50</v>
@@ -1282,7 +1257,7 @@
     </row>
     <row r="11" spans="1:11" s="4" customFormat="1">
       <c r="A11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>40</v>
@@ -1294,7 +1269,7 @@
         <v>0</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F11" s="4">
         <v>0.87968749999999996</v>
@@ -1317,7 +1292,7 @@
     </row>
     <row r="12" spans="1:11" s="4" customFormat="1">
       <c r="A12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>41</v>
@@ -1329,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F12" s="4">
         <v>0.876388888888888</v>
@@ -1352,7 +1327,7 @@
     </row>
     <row r="13" spans="1:11">
       <c r="A13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
@@ -1364,7 +1339,7 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F13">
         <v>0.89375000000000004</v>
@@ -1387,7 +1362,7 @@
     </row>
     <row r="14" spans="1:11">
       <c r="A14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
@@ -1399,7 +1374,7 @@
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14">
         <v>0.89375000000000004</v>
@@ -1422,7 +1397,7 @@
     </row>
     <row r="15" spans="1:11">
       <c r="A15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
@@ -1431,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
         <v>50</v>
@@ -1457,19 +1432,19 @@
     </row>
     <row r="16" spans="1:11" s="16" customFormat="1">
       <c r="A16" s="16" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="C16" s="17" t="b">
+        <v>0</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="16" t="s">
         <v>62</v>
-      </c>
-      <c r="C16" s="17" t="b">
-        <v>0</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="E16" s="16" t="s">
-        <v>63</v>
       </c>
       <c r="F16" s="16">
         <v>0.61666666666666603</v>
@@ -1492,19 +1467,19 @@
     </row>
     <row r="17" spans="1:11" s="16" customFormat="1">
       <c r="A17" s="16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C17" s="17" t="b">
         <v>0</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E17" s="16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F17" s="16">
         <v>1</v>
@@ -1527,19 +1502,19 @@
     </row>
     <row r="18" spans="1:11" s="16" customFormat="1">
       <c r="A18" s="16" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B18" s="16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C18" s="17" t="b">
         <v>0</v>
       </c>
       <c r="D18" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="16" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F18" s="16">
         <v>0.95833333333333304</v>
@@ -1562,7 +1537,7 @@
     </row>
     <row r="19" spans="1:11" s="9" customFormat="1">
       <c r="A19" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" s="9" t="s">
         <v>9</v>
@@ -1571,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>49</v>
@@ -1597,7 +1572,7 @@
     </row>
     <row r="20" spans="1:11" s="9" customFormat="1">
       <c r="A20" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B20" s="9" t="s">
         <v>10</v>
@@ -1606,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>50</v>
@@ -1632,7 +1607,7 @@
     </row>
     <row r="21" spans="1:11" s="9" customFormat="1">
       <c r="A21" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B21" s="9" t="s">
         <v>11</v>
@@ -1641,7 +1616,7 @@
         <v>0</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>49</v>
@@ -1667,7 +1642,7 @@
     </row>
     <row r="22" spans="1:11" s="9" customFormat="1">
       <c r="A22" s="9" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" s="9" t="s">
         <v>12</v>
@@ -1676,7 +1651,7 @@
         <v>0</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>50</v>
@@ -1702,7 +1677,7 @@
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
         <v>44</v>
@@ -1714,7 +1689,7 @@
         <v>0</v>
       </c>
       <c r="E23" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F23">
         <v>0.88854166666666601</v>
@@ -1737,7 +1712,7 @@
     </row>
     <row r="24" spans="1:11">
       <c r="A24" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
         <v>45</v>
@@ -1749,7 +1724,7 @@
         <v>0</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F24">
         <v>0.88888888888888895</v>
@@ -1772,7 +1747,7 @@
     </row>
     <row r="25" spans="1:11" s="7" customFormat="1">
       <c r="A25" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B25" s="7" t="s">
         <v>13</v>
@@ -1781,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>49</v>
@@ -1807,7 +1782,7 @@
     </row>
     <row r="26" spans="1:11" s="7" customFormat="1">
       <c r="A26" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B26" s="7" t="s">
         <v>14</v>
@@ -1816,7 +1791,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E26" s="7" t="s">
         <v>50</v>
@@ -1842,7 +1817,7 @@
     </row>
     <row r="27" spans="1:11" s="7" customFormat="1">
       <c r="A27" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="7" t="s">
         <v>15</v>
@@ -1851,7 +1826,7 @@
         <v>0</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E27" s="7" t="s">
         <v>49</v>
@@ -1877,7 +1852,7 @@
     </row>
     <row r="28" spans="1:11" s="7" customFormat="1">
       <c r="A28" s="7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B28" s="7" t="s">
         <v>16</v>
@@ -1886,7 +1861,7 @@
         <v>0</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E28" s="7" t="s">
         <v>50</v>
@@ -1912,7 +1887,7 @@
     </row>
     <row r="29" spans="1:11">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
         <v>46</v>
@@ -1924,7 +1899,7 @@
         <v>0</v>
       </c>
       <c r="E29" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F29">
         <v>0.89565972222222201</v>
@@ -1947,7 +1922,7 @@
     </row>
     <row r="30" spans="1:11">
       <c r="A30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" t="s">
         <v>47</v>
@@ -1959,7 +1934,7 @@
         <v>0</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F30">
         <v>0.89739583333333295</v>
@@ -1982,7 +1957,7 @@
     </row>
     <row r="31" spans="1:11" s="11" customFormat="1">
       <c r="A31" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>17</v>
@@ -1991,7 +1966,7 @@
         <v>0</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E31" s="11" t="s">
         <v>49</v>
@@ -2017,7 +1992,7 @@
     </row>
     <row r="32" spans="1:11" s="11" customFormat="1">
       <c r="A32" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>18</v>
@@ -2026,7 +2001,7 @@
         <v>0</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E32" s="11" t="s">
         <v>50</v>
@@ -2052,7 +2027,7 @@
     </row>
     <row r="33" spans="1:11" s="11" customFormat="1">
       <c r="A33" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B33" s="11" t="s">
         <v>19</v>
@@ -2061,7 +2036,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E33" s="11" t="s">
         <v>49</v>
@@ -2087,7 +2062,7 @@
     </row>
     <row r="34" spans="1:11" s="11" customFormat="1">
       <c r="A34" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B34" s="11" t="s">
         <v>20</v>
@@ -2096,7 +2071,7 @@
         <v>0</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E34" s="11" t="s">
         <v>50</v>
@@ -2122,7 +2097,7 @@
     </row>
     <row r="35" spans="1:11">
       <c r="A35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B35" t="s">
         <v>21</v>
@@ -2131,7 +2106,7 @@
         <v>0</v>
       </c>
       <c r="D35" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E35" t="s">
         <v>49</v>
@@ -2157,7 +2132,7 @@
     </row>
     <row r="36" spans="1:11">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B36" t="s">
         <v>22</v>
@@ -2166,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="D36" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E36" t="s">
         <v>50</v>
@@ -2192,7 +2167,7 @@
     </row>
     <row r="37" spans="1:11">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B37" t="s">
         <v>23</v>
@@ -2201,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="D37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E37" t="s">
         <v>49</v>
@@ -2227,7 +2202,7 @@
     </row>
     <row r="38" spans="1:11">
       <c r="A38" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B38" t="s">
         <v>24</v>
@@ -2236,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="D38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E38" t="s">
         <v>50</v>
@@ -2262,7 +2237,7 @@
     </row>
     <row r="39" spans="1:11">
       <c r="A39" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
@@ -2271,7 +2246,7 @@
         <v>1</v>
       </c>
       <c r="D39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E39" t="s">
         <v>49</v>
@@ -2297,7 +2272,7 @@
     </row>
     <row r="40" spans="1:11">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B40" t="s">
         <v>26</v>
@@ -2306,7 +2281,7 @@
         <v>1</v>
       </c>
       <c r="D40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E40" t="s">
         <v>50</v>
@@ -2332,7 +2307,7 @@
     </row>
     <row r="41" spans="1:11">
       <c r="A41" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B41" t="s">
         <v>27</v>
@@ -2341,7 +2316,7 @@
         <v>0</v>
       </c>
       <c r="D41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E41" t="s">
         <v>49</v>
@@ -2367,7 +2342,7 @@
     </row>
     <row r="42" spans="1:11">
       <c r="A42" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B42" t="s">
         <v>28</v>
@@ -2376,7 +2351,7 @@
         <v>0</v>
       </c>
       <c r="D42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E42" t="s">
         <v>50</v>
@@ -2402,7 +2377,7 @@
     </row>
     <row r="43" spans="1:11">
       <c r="A43" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
@@ -2411,7 +2386,7 @@
         <v>1</v>
       </c>
       <c r="D43" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E43" t="s">
         <v>49</v>
@@ -2437,7 +2412,7 @@
     </row>
     <row r="44" spans="1:11">
       <c r="A44" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
@@ -2446,7 +2421,7 @@
         <v>1</v>
       </c>
       <c r="D44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E44" t="s">
         <v>50</v>
@@ -2472,7 +2447,7 @@
     </row>
     <row r="45" spans="1:11">
       <c r="A45" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B45" t="s">
         <v>31</v>
@@ -2481,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="D45" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E45" t="s">
         <v>49</v>
@@ -2507,7 +2482,7 @@
     </row>
     <row r="46" spans="1:11">
       <c r="A46" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B46" t="s">
         <v>32</v>
@@ -2516,7 +2491,7 @@
         <v>0</v>
       </c>
       <c r="D46" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E46" t="s">
         <v>50</v>
@@ -2542,7 +2517,7 @@
     </row>
     <row r="47" spans="1:11">
       <c r="A47" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B47" t="s">
         <v>33</v>
@@ -2551,7 +2526,7 @@
         <v>1</v>
       </c>
       <c r="D47" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E47" t="s">
         <v>49</v>
@@ -2577,7 +2552,7 @@
     </row>
     <row r="48" spans="1:11">
       <c r="A48" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B48" t="s">
         <v>34</v>
@@ -2586,7 +2561,7 @@
         <v>1</v>
       </c>
       <c r="D48" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E48" t="s">
         <v>50</v>
@@ -2612,7 +2587,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B49" t="s">
         <v>35</v>
@@ -2621,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="D49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E49" t="s">
         <v>49</v>
@@ -2647,7 +2622,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B50" t="s">
         <v>36</v>
@@ -2656,7 +2631,7 @@
         <v>0</v>
       </c>
       <c r="D50" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E50" t="s">
         <v>50</v>
@@ -2682,7 +2657,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B51" t="s">
         <v>37</v>
@@ -2691,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="D51" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E51" t="s">
         <v>49</v>
@@ -2717,7 +2692,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B52" t="s">
         <v>38</v>
@@ -2726,7 +2701,7 @@
         <v>1</v>
       </c>
       <c r="D52" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E52" t="s">
         <v>50</v>
@@ -2752,74 +2727,69 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B53" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C53" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D53" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E53" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="54" spans="1:11">
       <c r="B54" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C54" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D54" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E54" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:11">
       <c r="B55" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C55" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D55" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E55" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="56" spans="1:11">
       <c r="B56" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C56" s="3" t="b">
         <v>0</v>
       </c>
       <c r="D56" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E56" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="1048575" spans="4:4">
       <c r="D1048575" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K56" xr:uid="{B9EF4E10-2359-3546-89E9-D98D539152BA}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K52">
-      <sortCondition ref="B1:B52"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K52">
     <sortCondition ref="B3:B52"/>
     <sortCondition descending="1" ref="F3:F52"/>
@@ -2830,7 +2800,7 @@
       <selection pane="bottomLeft" sqref="A1:A1048576"/>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
-      <autoFilter ref="A1:K56" xr:uid="{B9EF4E10-2359-3546-89E9-D98D539152BA}">
+      <autoFilter ref="A1:K56" xr:uid="{C2D8A03F-E774-B34D-820F-AD6CA59E8E85}">
         <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A4:K52">
           <sortCondition ref="B1:B52"/>
         </sortState>
@@ -2838,13 +2808,13 @@
     </customSheetView>
   </customSheetViews>
   <mergeCells count="7">
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="D1:D2"/>
     <mergeCell ref="C1:C2"/>
     <mergeCell ref="F1:G1"/>
     <mergeCell ref="H1:I1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="E1:E2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>